<commit_message>
Speech to Text Work Order Notes
</commit_message>
<xml_diff>
--- a/master_work_orders.xlsx
+++ b/master_work_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,6 +569,98 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11-17 12:59:02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WO-000002</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>#Vearthlyco2037</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Shipping</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CUS530</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>SPD</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>PPF - Insert</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>test 1 2 3 residual work order oh FedEx</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-17 12:59:02</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>WO-000002</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>#Vearthlyco2037</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Shipping</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CUS530</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>SPD</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>FAP - Amazon FBA Product Labeling</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>test 1 2 3 residual work order oh FedEx</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>